<commit_message>
Completed Part 2 practical
</commit_message>
<xml_diff>
--- a/Data/Excel/Keown_Excel-Practical_Part_2.xlsx
+++ b/Data/Excel/Keown_Excel-Practical_Part_2.xlsx
@@ -8,22 +8,41 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keown Naidoo\repos\sc_KeownNaidoo_2025\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{768C882C-1917-4E6E-8B78-6688CE9AC36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D306CE1-91F3-44C9-9A5D-DF528FAABF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Montgomery_Fleet_Equipment_Inve" sheetId="1" r:id="rId1"/>
+    <sheet name="Pivot1" sheetId="2" r:id="rId1"/>
+    <sheet name="Pivot2" sheetId="3" r:id="rId2"/>
+    <sheet name="Pivot3" sheetId="4" r:id="rId3"/>
+    <sheet name="Montgomery_Fleet_Equipment_Inve" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Montgomery_Fleet_Equipment_Inve!$A$1:$C$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Montgomery_Fleet_Equipment_Inve!$A$1:$C$50</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="6" r:id="rId5"/>
+  </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="37">
   <si>
     <t>Department</t>
   </si>
@@ -110,6 +129,30 @@
   </si>
   <si>
     <t>Off Road Vehicle Equipment</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>COUNT</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Equipment Count</t>
   </si>
 </sst>
 </file>
@@ -593,8 +636,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -651,6 +703,685 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Keown Naidoo" refreshedDate="45719.544021643516" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="49" xr:uid="{9651AEC7-FB60-437D-B053-26CA2C2BCD4A}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Department" numFmtId="0">
+      <sharedItems count="12">
+        <s v="Housing and Community Affairs"/>
+        <s v="Human Rights"/>
+        <s v="Libraries"/>
+        <s v="Liquor Control"/>
+        <s v="Office Of Homeland Security"/>
+        <s v="Permitting Services"/>
+        <s v="Public Information Office"/>
+        <s v="Recreation"/>
+        <s v="Sheriffs Office"/>
+        <s v="State Attorneys Office"/>
+        <s v="Technology Services"/>
+        <s v="Transportation"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Equipment Class" numFmtId="0">
+      <sharedItems count="14">
+        <s v="Pick Up Trucks"/>
+        <s v="SUV"/>
+        <s v="Sedan"/>
+        <s v="Van"/>
+        <s v="Medium Duty"/>
+        <s v="Heavy Duty"/>
+        <s v="CUV"/>
+        <s v="Off Road Vehicle Equipment"/>
+        <s v="Public Safety SUV"/>
+        <s v="Public Safety Van"/>
+        <s v="Public Safety CUV"/>
+        <s v="Public Safety Sedan"/>
+        <s v="Public Safety Pick Up Trucks"/>
+        <s v="Transit Bus"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Equipment Count" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="379"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="49">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="21"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="23"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <n v="42"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="6"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="27"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="24"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="48"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="2"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="0"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="3"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="7"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="8"/>
+    <n v="20"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="2"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="4"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="9"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="10"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="11"/>
+    <n v="46"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="12"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="11"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="3"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="1"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="2"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="6"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="3"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="1"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="0"/>
+    <n v="93"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="5"/>
+    <n v="248"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="13"/>
+    <n v="379"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="1"/>
+    <n v="53"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="3"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="4"/>
+    <n v="98"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="7"/>
+    <n v="276"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="6"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="2"/>
+    <n v="37"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{23D2A2B6-8B2A-44EC-ABE7-37D8AD10C0C6}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Equipment Count" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2315FD33-C5D1-4327-B9EC-B2476504E14A}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="13">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="10"/>
+        <item x="11"/>
+        <item t="default" sd="0"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="15">
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="7"/>
+        <item x="0"/>
+        <item x="10"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="13"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="22">
+    <i>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Equipment Count" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{22C89D03-EA81-4E74-AFFE-11B5E185ED13}" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="15">
+        <item x="6"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="10"/>
+        <item sd="0" x="12"/>
+        <item sd="0" x="11"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="9"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="13"/>
+        <item sd="0" x="3"/>
+        <item t="default" sd="0"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="18">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Equipment Count" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{439BEC4D-210D-4EEE-917F-F7C77E522FF4}" name="Table1" displayName="Table1" ref="A1:C50" totalsRowShown="0">
+  <autoFilter ref="A1:C50" xr:uid="{439BEC4D-210D-4EEE-917F-F7C77E522FF4}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{F8E2DDFF-152D-4919-989E-C91D0094C711}" name="Department"/>
+    <tableColumn id="2" xr3:uid="{13634DB4-1EA1-4CB2-B327-B88753125148}" name="Equipment Class"/>
+    <tableColumn id="3" xr3:uid="{8647DBFC-D536-4BD8-8562-0BDFC295596C}" name="Equipment Count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -949,19 +1680,526 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB7329B-A8D3-4D4C-950C-E68F30561C93}">
+  <dimension ref="A3:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1582</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64456C70-5E66-440E-AEF2-EB34E0DD61D1}">
+  <dimension ref="A3:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="4">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="4">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="4">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1582</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B566ACF9-A51C-4B85-8F7D-EF16D6DA2F31}">
+  <dimension ref="A3:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="4">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="4">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1582</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -972,7 +2210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -983,7 +2221,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -993,8 +2231,15 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3">
+        <f>SUM(C2:C50)</f>
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1004,8 +2249,15 @@
       <c r="C4">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1">
+        <f xml:space="preserve"> AVERAGE(C2:C50)</f>
+        <v>32.285714285714285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1015,8 +2267,15 @@
       <c r="C5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5">
+        <f>MIN(C2:C50)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1026,8 +2285,15 @@
       <c r="C6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6">
+        <f>MAX(C2:C50)</f>
+        <v>379</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1037,8 +2303,15 @@
       <c r="C7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7">
+        <f>COUNT(C2:C50)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1049,7 +2322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1060,7 +2333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1071,7 +2344,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1082,7 +2355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1093,7 +2366,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1104,7 +2377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1115,7 +2388,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1126,7 +2399,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1513,5 +2786,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>